<commit_message>
Sucess add 90.1183 / 90.1184 / 90.1185 / 90.1186
</commit_message>
<xml_diff>
--- a/Arif-0707/Arif-0707.xlsx
+++ b/Arif-0707/Arif-0707.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif-0707\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8096EE4-DDBB-48D4-9B29-A30AC429F065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325920FD-AD96-4064-BEB8-D6544E42B420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -403,7 +403,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -412,9 +412,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -778,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -814,302 +811,302 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="16" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:7" s="15" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="16" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:7" s="15" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="19" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:7" s="18" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="1:7" ht="34.5" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" s="11" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A5" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" s="16" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A6" s="13" t="s">
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+    </row>
+    <row r="6" spans="1:7" s="15" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:7" s="16" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A7" s="13" t="s">
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" s="15" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:7" s="16" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A8" s="13" t="s">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" s="15" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:7" s="9" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A9" s="6" t="s">
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" s="8" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="12" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:7" s="22" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A10" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:7" ht="34.5" customHeight="1">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" s="23" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A12" s="21" t="s">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" s="22" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A12" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="26"/>
-    </row>
-    <row r="13" spans="1:7" s="23" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A13" s="28" t="s">
+      <c r="F12" s="23"/>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="1:7" s="22" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A13" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="16" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:7" s="15" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A14" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" spans="1:7" s="16" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A15" s="13" t="s">
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:7" s="15" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A15" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="14"/>
-    </row>
-    <row r="16" spans="1:7" s="16" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A16" s="13" t="s">
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:7" s="15" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A16" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="14"/>
+      <c r="G16" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>